<commit_message>
changed git-mail - is it working now?
</commit_message>
<xml_diff>
--- a/time-records/Ertel_Bernhard.xlsx
+++ b/time-records/Ertel_Bernhard.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -68,6 +68,12 @@
     <t xml:space="preserve">Teammeeting</t>
   </si>
   <si>
+    <t xml:space="preserve">Implementierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update der Readme-files</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -90,9 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">Software/System Design und Architektur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementierung</t>
   </si>
   <si>
     <t xml:space="preserve">Tests</t>
@@ -352,7 +355,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,6 +420,15 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
         <v>44289</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6425,10 +6437,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6436,7 +6448,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6444,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6452,7 +6464,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6460,7 +6472,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6468,7 +6480,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6484,7 +6496,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6492,7 +6504,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6500,7 +6512,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6508,7 +6520,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
further test in the scenario and adaptation of Konzeptbeschreibung
</commit_message>
<xml_diff>
--- a/time-records/Ertel_Bernhard.xlsx
+++ b/time-records/Ertel_Bernhard.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -107,6 +107,18 @@
     <t xml:space="preserve">Präsentation Würfelkonfiguration</t>
   </si>
   <si>
+    <t xml:space="preserve">test for TermService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statusbesprechung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gameRoom erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">webSockets for gameRoom</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -141,13 +153,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="hh:mm"/>
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="169" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -259,7 +272,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +327,10 @@
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -404,10 +421,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.13"/>
@@ -633,31 +650,80 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="4" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="4" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="14" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A20" s="4" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B21" s="8" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="n">
+        <v>44323</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6542,12 +6608,16 @@
       <c r="D1005" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4 E8:E10 C15 C17:C20 C26:C1005" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4 E8:E10 C15 C17 C20 C26:C1005" type="list">
       <formula1>Tätigkeiten!$B$2:$B$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 C8 C11:C12 C14 C16" type="list">
+      <formula1>Tätigkeiten!$B$2:$B$12</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
       <formula1>Tätigkeiten!$B$2:$B$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6573,17 +6643,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>22</v>
+      <c r="A1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6591,7 +6661,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6599,7 +6669,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6607,7 +6677,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6615,7 +6685,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6623,7 +6693,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6639,7 +6709,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6655,7 +6725,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6663,7 +6733,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>